<commit_message>
Test for pin title on overlay
</commit_message>
<xml_diff>
--- a/excel-plist-data/Classroom lat_long plist data.xlsx
+++ b/excel-plist-data/Classroom lat_long plist data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjortberg521/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjortberg521/Desktop/SchoolMapper/excel-plist-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="23160" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="9780" yWindow="440" windowWidth="23160" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="130">
   <si>
     <t>001</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>Add at base of staircase - look during class</t>
+  </si>
+  <si>
+    <t>github commit test</t>
   </si>
 </sst>
 </file>
@@ -939,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P182"/>
+  <dimension ref="A1:P183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162:A163"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4682,7 +4685,7 @@
         <v>&lt;key&gt;035&lt;/key&gt;</v>
       </c>
       <c r="E138" s="16" t="str">
-        <f t="shared" ref="E138:E172" si="13">CONCATENATE("&lt;string&gt;",B138,"&lt;/string&gt;")</f>
+        <f t="shared" ref="E138:E161" si="13">CONCATENATE("&lt;string&gt;",B138,"&lt;/string&gt;")</f>
         <v>&lt;string&gt;42.089498&lt;/string&gt;</v>
       </c>
       <c r="I138" t="str">
@@ -5067,11 +5070,11 @@
         <v>&lt;string&gt;42.089675&lt;/string&gt;</v>
       </c>
       <c r="I152" t="str">
-        <f>CONCATENATE("let node", A151, " = ", "MyNode(name: ", """", A151, """)")</f>
+        <f t="shared" ref="I152:I162" si="14">CONCATENATE("let node", A151, " = ", "MyNode(name: ", """", A151, """)")</f>
         <v>let node048 = MyNode(name: "048")</v>
       </c>
       <c r="K152" s="4" t="str">
-        <f>CONCATENATE("node",A151,)</f>
+        <f t="shared" ref="K152:K162" si="15">CONCATENATE("node",A151,)</f>
         <v>node048</v>
       </c>
     </row>
@@ -5094,11 +5097,11 @@
         <v>&lt;string&gt;42.089055&lt;/string&gt;</v>
       </c>
       <c r="I153" t="str">
-        <f>CONCATENATE("let node", A152, " = ", "MyNode(name: ", """", A152, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node049 = MyNode(name: "049")</v>
       </c>
       <c r="K153" s="4" t="str">
-        <f>CONCATENATE("node",A152,)</f>
+        <f t="shared" si="15"/>
         <v>node049</v>
       </c>
     </row>
@@ -5121,11 +5124,11 @@
         <v>&lt;string&gt;42.089005&lt;/string&gt;</v>
       </c>
       <c r="I154" t="str">
-        <f>CONCATENATE("let node", A153, " = ", "MyNode(name: ", """", A153, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node050 = MyNode(name: "050")</v>
       </c>
       <c r="K154" s="4" t="str">
-        <f>CONCATENATE("node",A153,)</f>
+        <f t="shared" si="15"/>
         <v>node050</v>
       </c>
     </row>
@@ -5148,11 +5151,11 @@
         <v>&lt;string&gt;42.088679&lt;/string&gt;</v>
       </c>
       <c r="I155" t="str">
-        <f>CONCATENATE("let node", A154, " = ", "MyNode(name: ", """", A154, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node051 = MyNode(name: "051")</v>
       </c>
       <c r="K155" s="4" t="str">
-        <f>CONCATENATE("node",A154,)</f>
+        <f t="shared" si="15"/>
         <v>node051</v>
       </c>
     </row>
@@ -5175,11 +5178,11 @@
         <v>&lt;string&gt;42.088873&lt;/string&gt;</v>
       </c>
       <c r="I156" t="str">
-        <f>CONCATENATE("let node", A155, " = ", "MyNode(name: ", """", A155, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node052 = MyNode(name: "052")</v>
       </c>
       <c r="K156" s="4" t="str">
-        <f>CONCATENATE("node",A155,)</f>
+        <f t="shared" si="15"/>
         <v>node052</v>
       </c>
     </row>
@@ -5202,11 +5205,11 @@
         <v>&lt;string&gt;42.088545&lt;/string&gt;</v>
       </c>
       <c r="I157" t="str">
-        <f>CONCATENATE("let node", A156, " = ", "MyNode(name: ", """", A156, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node053 = MyNode(name: "053")</v>
       </c>
       <c r="K157" s="4" t="str">
-        <f>CONCATENATE("node",A156,)</f>
+        <f t="shared" si="15"/>
         <v>node053</v>
       </c>
     </row>
@@ -5229,11 +5232,11 @@
         <v>&lt;string&gt;42.088552&lt;/string&gt;</v>
       </c>
       <c r="I158" t="str">
-        <f>CONCATENATE("let node", A157, " = ", "MyNode(name: ", """", A157, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node054 = MyNode(name: "054")</v>
       </c>
       <c r="K158" s="4" t="str">
-        <f>CONCATENATE("node",A157,)</f>
+        <f t="shared" si="15"/>
         <v>node054</v>
       </c>
     </row>
@@ -5256,11 +5259,11 @@
         <v>&lt;string&gt;42.089857&lt;/string&gt;</v>
       </c>
       <c r="I159" t="str">
-        <f>CONCATENATE("let node", A158, " = ", "MyNode(name: ", """", A158, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node055 = MyNode(name: "055")</v>
       </c>
       <c r="K159" s="4" t="str">
-        <f>CONCATENATE("node",A158,)</f>
+        <f t="shared" si="15"/>
         <v>node055</v>
       </c>
     </row>
@@ -5275,7 +5278,7 @@
         <v>-87.851911999999999</v>
       </c>
       <c r="D160" s="18" t="str">
-        <f t="shared" ref="D160:D172" si="14">CONCATENATE("&lt;key&gt;",A160,"&lt;/key&gt;")</f>
+        <f t="shared" ref="D160:D163" si="16">CONCATENATE("&lt;key&gt;",A160,"&lt;/key&gt;")</f>
         <v>&lt;key&gt;057&lt;/key&gt;</v>
       </c>
       <c r="E160" s="16" t="str">
@@ -5283,11 +5286,11 @@
         <v>&lt;string&gt;42.08989&lt;/string&gt;</v>
       </c>
       <c r="I160" t="str">
-        <f>CONCATENATE("let node", A159, " = ", "MyNode(name: ", """", A159, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node056 = MyNode(name: "056")</v>
       </c>
       <c r="K160" s="4" t="str">
-        <f>CONCATENATE("node",A159,)</f>
+        <f t="shared" si="15"/>
         <v>node056</v>
       </c>
     </row>
@@ -5302,7 +5305,7 @@
         <v>-87.851915000000005</v>
       </c>
       <c r="D161" s="18" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>&lt;key&gt;058&lt;/key&gt;</v>
       </c>
       <c r="E161" s="16" t="str">
@@ -5310,11 +5313,11 @@
         <v>&lt;string&gt;42.089938&lt;/string&gt;</v>
       </c>
       <c r="I161" t="str">
-        <f>CONCATENATE("let node", A160, " = ", "MyNode(name: ", """", A160, """)")</f>
+        <f t="shared" si="14"/>
         <v>let node057 = MyNode(name: "057")</v>
       </c>
       <c r="K161" s="4" t="str">
-        <f>CONCATENATE("node",A160,)</f>
+        <f t="shared" si="15"/>
         <v>node057</v>
       </c>
     </row>
@@ -5323,15 +5326,15 @@
         <v>127</v>
       </c>
       <c r="D162" s="9" t="str">
+        <f t="shared" si="16"/>
+        <v>&lt;key&gt;Add more at the end of hallways&lt;/key&gt;</v>
+      </c>
+      <c r="I162" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;key&gt;Add more at the end of hallways&lt;/key&gt;</v>
-      </c>
-      <c r="I162" t="str">
-        <f>CONCATENATE("let node", A161, " = ", "MyNode(name: ", """", A161, """)")</f>
         <v>let node058 = MyNode(name: "058")</v>
       </c>
       <c r="K162" s="4" t="str">
-        <f>CONCATENATE("node",A161,)</f>
+        <f t="shared" si="15"/>
         <v>node058</v>
       </c>
     </row>
@@ -5340,7 +5343,7 @@
         <v>128</v>
       </c>
       <c r="D163" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>&lt;key&gt;Add at base of staircase - look during class&lt;/key&gt;</v>
       </c>
       <c r="F163" s="16"/>
@@ -5349,11 +5352,11 @@
     <row r="164" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="H164" s="4"/>
       <c r="I164" t="str">
-        <f>CONCATENATE("let node", A174, " = ", "MyNode(name: ", """", A174, """)")</f>
+        <f t="shared" ref="I164:I172" si="17">CONCATENATE("let node", A174, " = ", "MyNode(name: ", """", A174, """)")</f>
         <v>let node713 = MyNode(name: "713")</v>
       </c>
       <c r="K164" s="4" t="str">
-        <f>CONCATENATE("node",A174,)</f>
+        <f t="shared" ref="K164:K172" si="18">CONCATENATE("node",A174,)</f>
         <v>node713</v>
       </c>
     </row>
@@ -5362,11 +5365,11 @@
         <v>126</v>
       </c>
       <c r="I165" t="str">
-        <f>CONCATENATE("let node", A175, " = ", "MyNode(name: ", """", A175, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node715 = MyNode(name: "715")</v>
       </c>
       <c r="K165" s="4" t="str">
-        <f>CONCATENATE("node",A175,)</f>
+        <f t="shared" si="18"/>
         <v>node715</v>
       </c>
     </row>
@@ -5375,61 +5378,61 @@
         <v>125</v>
       </c>
       <c r="I166" t="str">
-        <f>CONCATENATE("let node", A176, " = ", "MyNode(name: ", """", A176, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node717 = MyNode(name: "717")</v>
       </c>
       <c r="K166" s="4" t="str">
-        <f>CONCATENATE("node",A176,)</f>
+        <f t="shared" si="18"/>
         <v>node717</v>
       </c>
     </row>
     <row r="167" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="I167" t="str">
-        <f>CONCATENATE("let node", A177, " = ", "MyNode(name: ", """", A177, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node712 = MyNode(name: "712")</v>
       </c>
       <c r="K167" s="4" t="str">
-        <f>CONCATENATE("node",A177,)</f>
+        <f t="shared" si="18"/>
         <v>node712</v>
       </c>
     </row>
     <row r="168" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="I168" t="str">
-        <f>CONCATENATE("let node", A178, " = ", "MyNode(name: ", """", A178, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node714 = MyNode(name: "714")</v>
       </c>
       <c r="K168" s="4" t="str">
-        <f>CONCATENATE("node",A178,)</f>
+        <f t="shared" si="18"/>
         <v>node714</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="I169" t="str">
-        <f>CONCATENATE("let node", A179, " = ", "MyNode(name: ", """", A179, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node742 = MyNode(name: "742")</v>
       </c>
       <c r="K169" s="4" t="str">
-        <f>CONCATENATE("node",A179,)</f>
+        <f t="shared" si="18"/>
         <v>node742</v>
       </c>
     </row>
     <row r="170" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="I170" t="str">
-        <f>CONCATENATE("let node", A180, " = ", "MyNode(name: ", """", A180, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node537 = MyNode(name: "537")</v>
       </c>
       <c r="K170" s="4" t="str">
-        <f>CONCATENATE("node",A180,)</f>
+        <f t="shared" si="18"/>
         <v>node537</v>
       </c>
     </row>
     <row r="171" spans="1:11" ht="13" x14ac:dyDescent="0.15">
       <c r="I171" t="str">
-        <f>CONCATENATE("let node", A181, " = ", "MyNode(name: ", """", A181, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node720 = MyNode(name: "720")</v>
       </c>
       <c r="K171" s="4" t="str">
-        <f>CONCATENATE("node",A181,)</f>
+        <f t="shared" si="18"/>
         <v>node720</v>
       </c>
     </row>
@@ -5447,15 +5450,15 @@
         <v>124</v>
       </c>
       <c r="E172" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B172,"&lt;/string&gt;")</f>
+        <f t="shared" ref="E172:E182" si="19">CONCATENATE("&lt;string&gt;",B172,"&lt;/string&gt;")</f>
         <v>&lt;string&gt;42.0886&lt;/string&gt;</v>
       </c>
       <c r="I172" t="str">
-        <f>CONCATENATE("let node", A182, " = ", "MyNode(name: ", """", A182, """)")</f>
+        <f t="shared" si="17"/>
         <v>let node710 = MyNode(name: "710")</v>
       </c>
       <c r="K172" s="4" t="str">
-        <f>CONCATENATE("node",A182,)</f>
+        <f t="shared" si="18"/>
         <v>node710</v>
       </c>
     </row>
@@ -5470,11 +5473,11 @@
         <v>-87.852054999999993</v>
       </c>
       <c r="D173" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A173,"&lt;/key&gt;")</f>
+        <f t="shared" ref="D173:D182" si="20">CONCATENATE("&lt;key&gt;",A173,"&lt;/key&gt;")</f>
         <v>&lt;key&gt;711&lt;/key&gt;</v>
       </c>
       <c r="E173" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B173,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089816&lt;/string&gt;</v>
       </c>
     </row>
@@ -5489,11 +5492,11 @@
         <v>-87.852119999999999</v>
       </c>
       <c r="D174" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A174,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;713&lt;/key&gt;</v>
       </c>
       <c r="E174" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B174,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089675&lt;/string&gt;</v>
       </c>
     </row>
@@ -5508,11 +5511,11 @@
         <v>-87.852154999999996</v>
       </c>
       <c r="D175" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A175,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;715&lt;/key&gt;</v>
       </c>
       <c r="E175" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B175,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089675&lt;/string&gt;</v>
       </c>
     </row>
@@ -5527,11 +5530,11 @@
         <v>-87.852310000000003</v>
       </c>
       <c r="D176" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A176,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;717&lt;/key&gt;</v>
       </c>
       <c r="E176" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B176,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089675&lt;/string&gt;</v>
       </c>
     </row>
@@ -5546,11 +5549,11 @@
         <v>-87.852339999999998</v>
       </c>
       <c r="D177" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A177,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;712&lt;/key&gt;</v>
       </c>
       <c r="E177" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B177,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089675&lt;/string&gt;</v>
       </c>
     </row>
@@ -5565,11 +5568,11 @@
         <v>-87.852683999999996</v>
       </c>
       <c r="D178" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A178,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;714&lt;/key&gt;</v>
       </c>
       <c r="E178" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B178,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089675&lt;/string&gt;</v>
       </c>
     </row>
@@ -5584,11 +5587,11 @@
         <v>-87.852739999999997</v>
       </c>
       <c r="D179" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A179,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;742&lt;/key&gt;</v>
       </c>
       <c r="E179" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B179,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089651&lt;/string&gt;</v>
       </c>
     </row>
@@ -5603,11 +5606,11 @@
         <v>-87.851985999999997</v>
       </c>
       <c r="D180" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A180,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;537&lt;/key&gt;</v>
       </c>
       <c r="E180" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B180,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089035&lt;/string&gt;</v>
       </c>
     </row>
@@ -5622,11 +5625,11 @@
         <v>-87.852014999999994</v>
       </c>
       <c r="D181" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A181,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;720&lt;/key&gt;</v>
       </c>
       <c r="E181" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B181,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.089992&lt;/string&gt;</v>
       </c>
     </row>
@@ -5641,12 +5644,17 @@
         <v>-87.851947999999993</v>
       </c>
       <c r="D182" s="18" t="str">
-        <f>CONCATENATE("&lt;key&gt;",A182,"&lt;/key&gt;")</f>
+        <f t="shared" si="20"/>
         <v>&lt;key&gt;710&lt;/key&gt;</v>
       </c>
       <c r="E182" s="16" t="str">
-        <f>CONCATENATE("&lt;string&gt;",B182,"&lt;/string&gt;")</f>
+        <f t="shared" si="19"/>
         <v>&lt;string&gt;42.090037&lt;/string&gt;</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A183" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>